<commit_message>
Creating a lisk of groups we may be able to partner with to develop a larger community of developers in the Tucson area.
</commit_message>
<xml_diff>
--- a/ProspectivePartnerGroups.xlsx
+++ b/ProspectivePartnerGroups.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
   <si>
     <r>
       <rPr>
@@ -283,6 +283,18 @@
   </si>
   <si>
     <t>Michelle</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/UAScienceLectures/</t>
+  </si>
+  <si>
+    <t>UA Science Lectures</t>
+  </si>
+  <si>
+    <t>The UA is hosting a bunch of computer science lectures at the start of 2018.</t>
+  </si>
+  <si>
+    <t>As of 1/19, looks like there are ~150 ppl signing up for each.</t>
   </si>
 </sst>
 </file>
@@ -339,13 +351,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -674,16 +686,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="5"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -742,10 +754,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43625C6-9F5F-4606-930A-1E417304B859}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,10 +811,10 @@
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D2" t="s">
@@ -865,10 +877,10 @@
       <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D5" t="s">
@@ -897,7 +909,7 @@
       <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E6">
@@ -960,7 +972,7 @@
       <c r="B9" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E9">
@@ -1057,6 +1069,23 @@
       </c>
       <c r="J13">
         <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated list with new meetup groups (and updated next meetup dates for some groups)
</commit_message>
<xml_diff>
--- a/ProspectivePartnerGroups.xlsx
+++ b/ProspectivePartnerGroups.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tech-exchange-for-civic-hackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBCEA8D-BA11-4F1B-AE46-F7CC2B9EE0A0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6190" activeTab="1" xr2:uid="{AA2F1323-3E90-4010-930F-1801CEE15F12}"/>
   </bookViews>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
   <si>
     <r>
       <rPr>
@@ -147,9 +148,6 @@
     <t>Tucson Python Meetup</t>
   </si>
   <si>
-    <t>1/23; 2/13</t>
-  </si>
-  <si>
     <t>Bi-monthly</t>
   </si>
   <si>
@@ -159,9 +157,6 @@
     <t>Google Developer Group</t>
   </si>
   <si>
-    <t>1/27;2/24</t>
-  </si>
-  <si>
     <t>Monthly</t>
   </si>
   <si>
@@ -177,9 +172,6 @@
     <t>Help researchers improve their development skills.</t>
   </si>
   <si>
-    <t>1/23; 1/25; 1/30</t>
-  </si>
-  <si>
     <t>Weekly</t>
   </si>
   <si>
@@ -216,9 +208,6 @@
     <t>They have had 40+ people signup for their last two events</t>
   </si>
   <si>
-    <t>None as of 1/19 but they just had one on 1/18.</t>
-  </si>
-  <si>
     <t>Infrequent Historically</t>
   </si>
   <si>
@@ -228,9 +217,6 @@
     <t>Tucson .NET User Group</t>
   </si>
   <si>
-    <t>2/21;</t>
-  </si>
-  <si>
     <t>https://www.meetup.com/Tucson-Adobe-User-Group/</t>
   </si>
   <si>
@@ -249,9 +235,6 @@
     <t>Tucson Functional Programmers</t>
   </si>
   <si>
-    <t>2/14; 3/14</t>
-  </si>
-  <si>
     <t>Montly</t>
   </si>
   <si>
@@ -295,6 +278,42 @@
   </si>
   <si>
     <t>As of 1/19, looks like there are ~150 ppl signing up for each.</t>
+  </si>
+  <si>
+    <t>3/8;</t>
+  </si>
+  <si>
+    <t>GDG Cloud Tucson</t>
+  </si>
+  <si>
+    <t>https://www.meetup.com/GDG-Cloud-Tucson/</t>
+  </si>
+  <si>
+    <t>3/13;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrew Slattery; </t>
+  </si>
+  <si>
+    <t>R-Ladies Tucson</t>
+  </si>
+  <si>
+    <t>https://www.meetup.com/rladies-tucson-az/</t>
+  </si>
+  <si>
+    <t>[Summarized from meetup desc] Promote gender diversity in the R statistical computing community. All events are intended for women but men are welcome to attend as a guest.</t>
+  </si>
+  <si>
+    <t>Adriana Picoral;</t>
+  </si>
+  <si>
+    <t>3/15;</t>
+  </si>
+  <si>
+    <t>3/20;</t>
+  </si>
+  <si>
+    <t>3/22;</t>
   </si>
 </sst>
 </file>
@@ -754,10 +773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43625C6-9F5F-4606-930A-1E417304B859}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,7 +799,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>12</v>
@@ -815,7 +834,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -838,7 +857,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -858,16 +877,16 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="E4">
         <v>429</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -875,25 +894,25 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="E5">
         <v>818</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -901,22 +920,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="E6">
         <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -924,13 +943,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -944,36 +963,36 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="E8">
         <v>781</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J8">
         <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="E9">
         <v>95</v>
@@ -984,16 +1003,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>378</v>
@@ -1004,36 +1023,36 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="D11" s="4">
+        <v>43173</v>
       </c>
       <c r="E11">
         <v>487</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E12">
         <v>48</v>
@@ -1042,30 +1061,30 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E13">
         <v>102</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J13">
         <v>2</v>
@@ -1073,19 +1092,56 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16">
+        <v>85</v>
+      </c>
+      <c r="G16" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>